<commit_message>
tons of work on drought array MS that I got lazy about logging
</commit_message>
<xml_diff>
--- a/PuertoRico-Field-Materials/Reimbursements/2016-Jan-PRtrip/reimbursement-tracking-2016-Jan-PRtrip.xlsx
+++ b/PuertoRico-Field-Materials/Reimbursements/2016-Jan-PRtrip/reimbursement-tracking-2016-Jan-PRtrip.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="460" windowWidth="18000" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="1660" yWindow="1460" windowWidth="18000" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>Super Shuttle from SFO</t>
+  </si>
+  <si>
+    <t>Bag fee on Jet Blue</t>
   </si>
 </sst>
 </file>
@@ -193,11 +199,11 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,7 +485,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,49 +497,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="9"/>
       <c r="C2">
         <v>12840622</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>23</v>
       </c>
@@ -543,10 +549,10 @@
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -561,10 +567,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
@@ -624,10 +630,10 @@
       <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="8">
         <v>346.3</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -636,10 +642,10 @@
       <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="8">
         <v>181.31</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -648,8 +654,8 @@
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
       <c r="I17">
         <v>30.58</v>
       </c>
@@ -661,8 +667,8 @@
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8">
         <v>41</v>
       </c>
     </row>
@@ -673,8 +679,8 @@
       <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8">
         <v>100</v>
       </c>
     </row>
@@ -685,8 +691,8 @@
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
       <c r="I20">
         <v>50</v>
       </c>
@@ -695,8 +701,8 @@
       <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="I21">
         <v>22</v>
       </c>
@@ -708,9 +714,20 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8">
         <v>41.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>42390</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>